<commit_message>
Preparing objects necessary for algorithm development.
</commit_message>
<xml_diff>
--- a/direct_join_prepared.xlsx
+++ b/direct_join_prepared.xlsx
@@ -1,60 +1,66 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Documents/GitHub/YouScience/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F296DF2-A1DD-F743-9A04-64F980FACE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="22260" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="83">
   <si>
     <t>YouScience Clusters</t>
   </si>
   <si>
+    <t>Oakland Middle School</t>
+  </si>
+  <si>
+    <t>Siegel Middle School</t>
+  </si>
+  <si>
+    <t>Whitworth-Buchanan Middle School</t>
+  </si>
+  <si>
+    <t>Christiana Middle School</t>
+  </si>
+  <si>
+    <t>Smyrna Middle School</t>
+  </si>
+  <si>
+    <t>Stewarts Creek Middle School</t>
+  </si>
+  <si>
+    <t>Rockvale Middle School</t>
+  </si>
+  <si>
+    <t>Rocky Fork Middle School</t>
+  </si>
+  <si>
     <t>Blackman Middle School</t>
   </si>
   <si>
-    <t>Christiana Middle School</t>
+    <t>Thurman Francis Arts Academy</t>
+  </si>
+  <si>
+    <t>Rock Springs Middle School</t>
   </si>
   <si>
     <t>LaVergne Middle School</t>
   </si>
   <si>
-    <t>Oakland Middle School</t>
-  </si>
-  <si>
-    <t>Rock Springs Middle School</t>
-  </si>
-  <si>
-    <t>Rockvale Middle School</t>
-  </si>
-  <si>
-    <t>Rocky Fork Middle School</t>
-  </si>
-  <si>
-    <t>Siegel Middle School</t>
-  </si>
-  <si>
-    <t>Smyrna Middle School</t>
-  </si>
-  <si>
-    <t>Stewarts Creek Middle School</t>
-  </si>
-  <si>
-    <t>Thurman Francis Arts Academy</t>
-  </si>
-  <si>
-    <t>Whitworth-Buchanan Middle School</t>
-  </si>
-  <si>
     <t>Business</t>
   </si>
   <si>
@@ -101,12 +107,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Human Services</t>
-  </si>
-  <si>
-    <t>Smryna &amp; Therman Francis-&gt; Smyrna HS</t>
-  </si>
-  <si>
-    <t>Christiana &amp; Whitworth -&gt; Riverdale</t>
   </si>
   <si>
     <t>Business Management</t>
@@ -274,8 +274,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +338,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -384,7 +392,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,9 +424,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -450,6 +476,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -625,14 +669,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="87.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="99" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="99" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="63.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -681,31 +743,31 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -713,43 +775,43 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -757,34 +819,34 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -792,40 +854,40 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -833,28 +895,28 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -862,22 +924,22 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -885,7 +947,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -893,43 +955,43 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="M9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -937,43 +999,43 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -981,19 +1043,19 @@
         <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1001,34 +1063,34 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1036,40 +1098,40 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1077,43 +1139,43 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1121,22 +1183,22 @@
         <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1144,43 +1206,43 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1188,113 +1250,40 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="C18">
-        <v>4</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-      <c r="E18">
-        <v>8</v>
-      </c>
-      <c r="F18">
-        <v>3</v>
-      </c>
-      <c r="G18">
-        <v>4</v>
-      </c>
-      <c r="H18">
-        <v>3</v>
-      </c>
-      <c r="I18">
-        <v>3</v>
-      </c>
-      <c r="J18">
-        <v>4</v>
-      </c>
-      <c r="K18">
-        <v>3</v>
-      </c>
-      <c r="L18">
-        <v>4</v>
-      </c>
-      <c r="M18">
-        <v>3</v>
-      </c>
-      <c r="N18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="C20">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Template for student schedules created. Next step automation throughout county
</commit_message>
<xml_diff>
--- a/direct_join_prepared.xlsx
+++ b/direct_join_prepared.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Documents/GitHub/YouScience/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F955304B-A0B2-1946-A666-63B55AD86838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2660" yWindow="760" windowWidth="21080" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -100,9 +106,6 @@
     <t>Government &amp; Public Admin</t>
   </si>
   <si>
-    <t xml:space="preserve"> Human Services</t>
-  </si>
-  <si>
     <t>Smryna &amp; Therman Francis-&gt; Smyrna HS</t>
   </si>
   <si>
@@ -269,13 +272,16 @@
   </si>
   <si>
     <t>Cosmetology</t>
+  </si>
+  <si>
+    <t>Human Services</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +344,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -384,7 +398,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,9 +430,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -450,6 +482,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -625,14 +675,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="87.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +728,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -681,31 +736,31 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -713,43 +768,43 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -757,34 +812,34 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -792,40 +847,40 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -833,28 +888,28 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -862,22 +917,22 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -885,7 +940,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -893,43 +948,43 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -937,43 +992,43 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -981,19 +1036,19 @@
         <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1001,34 +1056,34 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1036,40 +1091,40 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1077,43 +1132,43 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1121,22 +1176,22 @@
         <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1144,87 +1199,87 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1265,7 +1320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1273,7 +1328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1281,20 +1336,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Begun refactoring into beta_algorithm_v1.ipynb. Approx. 25% done.
</commit_message>
<xml_diff>
--- a/direct_join_prepared.xlsx
+++ b/direct_join_prepared.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Documents/GitHub/YouScience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F955304B-A0B2-1946-A666-63B55AD86838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8498EA-78D3-B84C-911E-AB5D2D6863B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2660" yWindow="760" windowWidth="21080" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="83">
   <si>
     <t>YouScience Clusters</t>
   </si>
@@ -106,12 +119,6 @@
     <t>Government &amp; Public Admin</t>
   </si>
   <si>
-    <t>Smryna &amp; Therman Francis-&gt; Smyrna HS</t>
-  </si>
-  <si>
-    <t>Christiana &amp; Whitworth -&gt; Riverdale</t>
-  </si>
-  <si>
     <t>Business Management</t>
   </si>
   <si>
@@ -187,9 +194,6 @@
     <t>Residential &amp; Commercial Construction</t>
   </si>
   <si>
-    <t>BioSTEM, Dietetics &amp; Nutrition, Veterinary &amp; Animal Science/Horticulture Science, Sport &amp; Human Performance</t>
-  </si>
-  <si>
     <t>Mechantronics</t>
   </si>
   <si>
@@ -275,6 +279,9 @@
   </si>
   <si>
     <t>Human Services</t>
+  </si>
+  <si>
+    <t>BioSTEM, Dietetics &amp; Nutrition, Sport &amp; Human Performance</t>
   </si>
 </sst>
 </file>
@@ -356,7 +363,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -676,15 +683,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="87.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="99" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="99" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="63.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -736,28 +756,28 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="N2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -768,40 +788,40 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -812,31 +832,31 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -847,37 +867,37 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="M5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -888,25 +908,25 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -917,19 +937,19 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -948,40 +968,40 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -992,40 +1012,40 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -1036,16 +1056,16 @@
         <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -1056,31 +1076,31 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -1091,37 +1111,37 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -1132,40 +1152,40 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="N14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -1176,19 +1196,19 @@
         <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1199,40 +1219,40 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -1240,116 +1260,43 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="C18">
-        <v>4</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-      <c r="E18">
-        <v>8</v>
-      </c>
-      <c r="F18">
-        <v>3</v>
-      </c>
-      <c r="G18">
-        <v>4</v>
-      </c>
-      <c r="H18">
-        <v>3</v>
-      </c>
-      <c r="I18">
-        <v>3</v>
-      </c>
-      <c r="J18">
-        <v>4</v>
-      </c>
-      <c r="K18">
-        <v>3</v>
-      </c>
-      <c r="L18">
-        <v>4</v>
-      </c>
-      <c r="M18">
-        <v>3</v>
-      </c>
-      <c r="N18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="C20">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>